<commit_message>
Exp2 fixes and first runs
</commit_message>
<xml_diff>
--- a/Results/horse-colic_results.xlsx
+++ b/Results/horse-colic_results.xlsx
@@ -495,34 +495,34 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>13.7037037037037</v>
+        <v>12.22222222222222</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4814814814814815</v>
+        <v>0.3703703703703703</v>
       </c>
       <c r="D2" t="n">
-        <v>99.62962962962962</v>
+        <v>99.66666666666667</v>
       </c>
       <c r="E2" t="n">
-        <v>33.33333333333334</v>
+        <v>30</v>
       </c>
       <c r="F2" t="n">
-        <v>4.888888888888888</v>
+        <v>5.259259259259259</v>
       </c>
       <c r="G2" t="n">
-        <v>32.62962962962963</v>
+        <v>34.96296296296296</v>
       </c>
       <c r="H2" t="n">
-        <v>67.37037037037037</v>
+        <v>69.14814814814814</v>
       </c>
       <c r="I2" t="n">
-        <v>21.92592592592593</v>
+        <v>19.92592592592593</v>
       </c>
       <c r="J2" t="n">
-        <v>24.2962962962963</v>
+        <v>21.07407407407408</v>
       </c>
       <c r="K2" t="n">
-        <v>31.30541486448114</v>
+        <v>26.13121201216228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>